<commit_message>
Added tag options TotalLabel and GrandLabel for Group tag
</commit_message>
<xml_diff>
--- a/tests/Gauges/GroupTagTests_Simple.xlsx
+++ b/tests/Gauges/GroupTagTests_Simple.xlsx
@@ -90,22 +90,22 @@
     <x:t>Check</x:t>
   </x:si>
   <x:si>
-    <x:t>Check Total</x:t>
+    <x:t>Check SUM</x:t>
   </x:si>
   <x:si>
     <x:t>Credit</x:t>
   </x:si>
   <x:si>
-    <x:t>Credit Total</x:t>
+    <x:t>Credit SUM</x:t>
   </x:si>
   <x:si>
     <x:t>Visa</x:t>
   </x:si>
   <x:si>
-    <x:t>Visa Total</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Общий Total</x:t>
+    <x:t>Visa SUM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>By All SUM</x:t>
   </x:si>
   <x:si>
     <x:t>Phone</x:t>
@@ -340,18 +340,30 @@
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="3" fontId="0" fillId="0" borderId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="164" fontId="0" fillId="0" borderId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="0" fillId="0" borderId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
     <x:xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
     <x:xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -389,18 +401,6 @@
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="13" fillId="2" borderId="4" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="3" fontId="0" fillId="0" borderId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="164" fontId="0" fillId="0" borderId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="4" fontId="0" fillId="0" borderId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="2" fillId="0" borderId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -550,46 +550,62 @@
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="3" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="4" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
     <x:xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
     <x:xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="2" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
@@ -644,22 +660,6 @@
     </x:xf>
     <x:xf numFmtId="0" fontId="13" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="3" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="4" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1184,8 +1184,8 @@
   <x:sheetViews>
     <x:sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <x:pane xSplit="0" ySplit="11" topLeftCell="A12" activePane="bottomLeft" state="frozenSplit"/>
-      <x:selection activeCell="L4" sqref="L4"/>
-      <x:selection pane="bottomLeft" activeCell="L4" sqref="L4"/>
+      <x:selection activeCell="G13" sqref="G13"/>
+      <x:selection pane="bottomLeft" activeCell="G13" sqref="G13"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="11.25" outlineLevelCol="2"/>
@@ -1203,51 +1203,51 @@
     <x:col min="11" max="11" width="9.140625" style="50" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:12" customFormat="1" ht="51" customHeight="1">
+    <x:row r="1" spans="1:11" customFormat="1" ht="51" customHeight="1">
       <x:c r="A1" s="50" t="s"/>
-      <x:c r="B1" s="52" t="s">
+      <x:c r="B1" s="55" t="s">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="C1" s="53" t="s"/>
-      <x:c r="D1" s="53" t="s"/>
-      <x:c r="E1" s="53" t="s"/>
-      <x:c r="F1" s="53" t="s"/>
-      <x:c r="G1" s="53" t="s"/>
-      <x:c r="H1" s="53" t="s"/>
-      <x:c r="I1" s="53" t="s"/>
-      <x:c r="J1" s="53" t="s"/>
-    </x:row>
-    <x:row r="2" spans="1:12" customFormat="1" ht="12.75" customHeight="1">
+      <x:c r="C1" s="56" t="s"/>
+      <x:c r="D1" s="56" t="s"/>
+      <x:c r="E1" s="56" t="s"/>
+      <x:c r="F1" s="56" t="s"/>
+      <x:c r="G1" s="56" t="s"/>
+      <x:c r="H1" s="56" t="s"/>
+      <x:c r="I1" s="56" t="s"/>
+      <x:c r="J1" s="56" t="s"/>
+    </x:row>
+    <x:row r="2" spans="1:11" customFormat="1" ht="12.75" customHeight="1">
       <x:c r="A2" s="50" t="s"/>
-      <x:c r="B2" s="54" t="s"/>
-      <x:c r="C2" s="54" t="s"/>
-      <x:c r="D2" s="54" t="s"/>
-      <x:c r="E2" s="54" t="s"/>
-      <x:c r="F2" s="54" t="s"/>
-      <x:c r="G2" s="54" t="s"/>
-      <x:c r="H2" s="54" t="s"/>
-      <x:c r="I2" s="54" t="s"/>
+      <x:c r="B2" s="57" t="s"/>
+      <x:c r="C2" s="57" t="s"/>
+      <x:c r="D2" s="57" t="s"/>
+      <x:c r="E2" s="57" t="s"/>
+      <x:c r="F2" s="57" t="s"/>
+      <x:c r="G2" s="57" t="s"/>
+      <x:c r="H2" s="57" t="s"/>
+      <x:c r="I2" s="57" t="s"/>
       <x:c r="J2" s="50" t="s"/>
     </x:row>
-    <x:row r="3" spans="1:12" customFormat="1" ht="18" customHeight="1">
-      <x:c r="A3" s="55" t="s"/>
-      <x:c r="B3" s="56" t="s">
+    <x:row r="3" spans="1:11" customFormat="1" ht="18" customHeight="1">
+      <x:c r="A3" s="58" t="s"/>
+      <x:c r="B3" s="59" t="s">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="C3" s="57" t="s">
+      <x:c r="C3" s="60" t="s">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="D3" s="58" t="s"/>
-      <x:c r="E3" s="58" t="s"/>
-      <x:c r="F3" s="58" t="s"/>
-      <x:c r="G3" s="59" t="s"/>
-      <x:c r="H3" s="59" t="s"/>
-      <x:c r="I3" s="59" t="s"/>
-      <x:c r="J3" s="60" t="s"/>
-    </x:row>
-    <x:row r="4" spans="1:12">
+      <x:c r="D3" s="61" t="s"/>
+      <x:c r="E3" s="61" t="s"/>
+      <x:c r="F3" s="61" t="s"/>
+      <x:c r="G3" s="62" t="s"/>
+      <x:c r="H3" s="62" t="s"/>
+      <x:c r="I3" s="62" t="s"/>
+      <x:c r="J3" s="63" t="s"/>
+    </x:row>
+    <x:row r="4" spans="1:11">
       <x:c r="A4" s="50" t="s"/>
-      <x:c r="B4" s="51" t="s"/>
+      <x:c r="B4" s="64" t="s"/>
       <x:c r="C4" s="50" t="s"/>
       <x:c r="D4" s="50" t="s"/>
       <x:c r="E4" s="50" t="s"/>
@@ -1257,169 +1257,169 @@
       <x:c r="I4" s="50" t="s"/>
       <x:c r="J4" s="50" t="s"/>
     </x:row>
-    <x:row r="5" spans="1:12">
+    <x:row r="5" spans="1:11">
       <x:c r="A5" s="50" t="s"/>
-      <x:c r="B5" s="56" t="s">
+      <x:c r="B5" s="59" t="s">
         <x:v>3</x:v>
       </x:c>
       <x:c r="C5" s="50" t="s"/>
     </x:row>
-    <x:row r="6" spans="1:12" customFormat="1" ht="12" customHeight="1">
+    <x:row r="6" spans="1:11" customFormat="1" ht="12" customHeight="1">
       <x:c r="A6" s="50" t="s"/>
-      <x:c r="B6" s="61" t="s">
+      <x:c r="B6" s="65" t="s">
         <x:f>"4-976 Sugarloaf Hwy"&amp;" "&amp;"Suite 103"</x:f>
       </x:c>
-      <x:c r="C6" s="62" t="s"/>
-      <x:c r="D6" s="62" t="s"/>
-      <x:c r="E6" s="62" t="s"/>
-      <x:c r="F6" s="62" t="s"/>
-      <x:c r="G6" s="62" t="s"/>
-      <x:c r="H6" s="63" t="s"/>
-      <x:c r="I6" s="64" t="s"/>
-      <x:c r="J6" s="65" t="s"/>
-    </x:row>
-    <x:row r="7" spans="1:12" customFormat="1" ht="12" customHeight="1">
+      <x:c r="C6" s="66" t="s"/>
+      <x:c r="D6" s="66" t="s"/>
+      <x:c r="E6" s="66" t="s"/>
+      <x:c r="F6" s="66" t="s"/>
+      <x:c r="G6" s="66" t="s"/>
+      <x:c r="H6" s="67" t="s"/>
+      <x:c r="I6" s="68" t="s"/>
+      <x:c r="J6" s="69" t="s"/>
+    </x:row>
+    <x:row r="7" spans="1:11" customFormat="1" ht="12" customHeight="1">
       <x:c r="A7" s="50" t="s"/>
-      <x:c r="B7" s="66" t="s"/>
-      <x:c r="C7" s="67" t="s"/>
-      <x:c r="D7" s="67" t="s"/>
-      <x:c r="E7" s="67" t="s"/>
-      <x:c r="F7" s="67" t="s"/>
-      <x:c r="G7" s="67" t="s"/>
-      <x:c r="H7" s="66" t="s"/>
+      <x:c r="B7" s="70" t="s"/>
+      <x:c r="C7" s="71" t="s"/>
+      <x:c r="D7" s="71" t="s"/>
+      <x:c r="E7" s="71" t="s"/>
+      <x:c r="F7" s="71" t="s"/>
+      <x:c r="G7" s="71" t="s"/>
+      <x:c r="H7" s="70" t="s"/>
       <x:c r="I7" s="50" t="s"/>
       <x:c r="J7" s="50" t="s"/>
     </x:row>
-    <x:row r="8" spans="1:12">
+    <x:row r="8" spans="1:11">
       <x:c r="A8" s="50" t="s"/>
-      <x:c r="B8" s="56" t="s">
+      <x:c r="B8" s="59" t="s">
         <x:v>4</x:v>
       </x:c>
-      <x:c r="E8" s="56" t="s">
+      <x:c r="E8" s="59" t="s">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="G8" s="56" t="s">
+      <x:c r="G8" s="59" t="s">
         <x:v>6</x:v>
       </x:c>
-      <x:c r="I8" s="56" t="s">
+      <x:c r="I8" s="59" t="s">
         <x:v>7</x:v>
       </x:c>
     </x:row>
-    <x:row r="9" spans="1:12" customFormat="1" ht="12" customHeight="1">
+    <x:row r="9" spans="1:11" customFormat="1" ht="12" customHeight="1">
       <x:c r="A9" s="50" t="s"/>
-      <x:c r="B9" s="68" t="s">
+      <x:c r="B9" s="72" t="s">
         <x:v>8</x:v>
       </x:c>
-      <x:c r="C9" s="62" t="s"/>
-      <x:c r="D9" s="62" t="s"/>
-      <x:c r="E9" s="68" t="s">
+      <x:c r="C9" s="66" t="s"/>
+      <x:c r="D9" s="66" t="s"/>
+      <x:c r="E9" s="72" t="s">
         <x:v>9</x:v>
       </x:c>
-      <x:c r="F9" s="69" t="s"/>
-      <x:c r="G9" s="68" t="s">
+      <x:c r="F9" s="73" t="s"/>
+      <x:c r="G9" s="72" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="H9" s="69" t="s"/>
-      <x:c r="I9" s="68" t="s">
+      <x:c r="H9" s="73" t="s"/>
+      <x:c r="I9" s="72" t="s">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="J9" s="69" t="s"/>
-    </x:row>
-    <x:row r="10" spans="1:12" customFormat="1" ht="12" customHeight="1">
+      <x:c r="J9" s="73" t="s"/>
+    </x:row>
+    <x:row r="10" spans="1:11" customFormat="1" ht="12" customHeight="1">
       <x:c r="A10" s="50" t="s"/>
-      <x:c r="B10" s="70" t="s"/>
-      <x:c r="C10" s="67" t="s"/>
-      <x:c r="D10" s="67" t="s"/>
-      <x:c r="E10" s="70" t="s"/>
-      <x:c r="F10" s="67" t="s"/>
-      <x:c r="G10" s="70" t="s"/>
-      <x:c r="H10" s="67" t="s"/>
-      <x:c r="I10" s="70" t="s"/>
-      <x:c r="J10" s="67" t="s"/>
-    </x:row>
-    <x:row r="11" spans="1:12" customFormat="1" ht="22.5" customHeight="1">
+      <x:c r="B10" s="74" t="s"/>
+      <x:c r="C10" s="71" t="s"/>
+      <x:c r="D10" s="71" t="s"/>
+      <x:c r="E10" s="74" t="s"/>
+      <x:c r="F10" s="71" t="s"/>
+      <x:c r="G10" s="74" t="s"/>
+      <x:c r="H10" s="71" t="s"/>
+      <x:c r="I10" s="74" t="s"/>
+      <x:c r="J10" s="71" t="s"/>
+    </x:row>
+    <x:row r="11" spans="1:11" customFormat="1" ht="22.5" customHeight="1">
       <x:c r="A11" s="50" t="s"/>
-      <x:c r="B11" s="71" t="s">
+      <x:c r="B11" s="75" t="s">
         <x:v>12</x:v>
       </x:c>
-      <x:c r="C11" s="72" t="s">
+      <x:c r="C11" s="76" t="s">
         <x:v>13</x:v>
       </x:c>
-      <x:c r="D11" s="71" t="s">
+      <x:c r="D11" s="75" t="s">
         <x:v>14</x:v>
       </x:c>
-      <x:c r="E11" s="71" t="s">
+      <x:c r="E11" s="75" t="s">
         <x:v>15</x:v>
       </x:c>
-      <x:c r="F11" s="71" t="s">
+      <x:c r="F11" s="75" t="s">
         <x:v>16</x:v>
       </x:c>
-      <x:c r="G11" s="73" t="s">
+      <x:c r="G11" s="77" t="s">
         <x:v>17</x:v>
       </x:c>
-      <x:c r="H11" s="74" t="s">
+      <x:c r="H11" s="78" t="s">
         <x:v>18</x:v>
       </x:c>
-      <x:c r="I11" s="74" t="s">
+      <x:c r="I11" s="78" t="s">
         <x:v>19</x:v>
       </x:c>
-      <x:c r="J11" s="74" t="s">
+      <x:c r="J11" s="78" t="s">
         <x:v>20</x:v>
       </x:c>
     </x:row>
-    <x:row r="12" spans="1:12" outlineLevel="2">
+    <x:row r="12" spans="1:11" outlineLevel="2">
       <x:c r="A12" s="50" t="s"/>
-      <x:c r="B12" s="75" t="n">
+      <x:c r="B12" s="52" t="n">
         <x:v>1023</x:v>
       </x:c>
-      <x:c r="C12" s="76">
+      <x:c r="C12" s="53">
         <x:v>32325</x:v>
       </x:c>
-      <x:c r="D12" s="76">
+      <x:c r="D12" s="53">
         <x:v>32326</x:v>
       </x:c>
-      <x:c r="E12" s="77" t="s"/>
-      <x:c r="F12" s="77" t="s"/>
-      <x:c r="G12" s="77" t="s">
+      <x:c r="E12" s="51" t="s"/>
+      <x:c r="F12" s="51" t="s"/>
+      <x:c r="G12" s="51" t="s">
         <x:v>21</x:v>
       </x:c>
-      <x:c r="H12" s="78" t="n">
+      <x:c r="H12" s="54" t="n">
         <x:v>4674</x:v>
       </x:c>
-      <x:c r="I12" s="78" t="n">
+      <x:c r="I12" s="54" t="n">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="J12" s="78" t="n">
+      <x:c r="J12" s="54" t="n">
         <x:v>4674</x:v>
       </x:c>
     </x:row>
-    <x:row r="13" spans="1:12" outlineLevel="2">
+    <x:row r="13" spans="1:11" outlineLevel="2">
       <x:c r="A13" s="50" t="s"/>
-      <x:c r="B13" s="75" t="n">
+      <x:c r="B13" s="52" t="n">
         <x:v>1123</x:v>
       </x:c>
-      <x:c r="C13" s="76">
+      <x:c r="C13" s="53">
         <x:v>34205</x:v>
       </x:c>
-      <x:c r="D13" s="76">
+      <x:c r="D13" s="53">
         <x:v>34205</x:v>
       </x:c>
-      <x:c r="E13" s="77" t="s"/>
-      <x:c r="F13" s="77" t="s"/>
-      <x:c r="G13" s="77" t="s">
+      <x:c r="E13" s="51" t="s"/>
+      <x:c r="F13" s="51" t="s"/>
+      <x:c r="G13" s="51" t="s">
         <x:v>21</x:v>
       </x:c>
-      <x:c r="H13" s="78" t="n">
+      <x:c r="H13" s="54" t="n">
         <x:v>13945</x:v>
       </x:c>
-      <x:c r="I13" s="78" t="n">
+      <x:c r="I13" s="54" t="n">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="J13" s="78" t="n">
+      <x:c r="J13" s="54" t="n">
         <x:v>13945</x:v>
       </x:c>
     </x:row>
-    <x:row r="14" spans="1:12" outlineLevel="1">
+    <x:row r="14" spans="1:11" outlineLevel="1">
       <x:c r="A14" s="50" t="s"/>
       <x:c r="B14" s="82" t="s"/>
       <x:c r="C14" s="83" t="s"/>
@@ -1437,59 +1437,59 @@
         <x:f>Subtotal(9,J12:J13)</x:f>
       </x:c>
     </x:row>
-    <x:row r="15" spans="1:12" outlineLevel="2">
+    <x:row r="15" spans="1:11" outlineLevel="2">
       <x:c r="A15" s="50" t="s"/>
-      <x:c r="B15" s="75" t="n">
+      <x:c r="B15" s="52" t="n">
         <x:v>1269</x:v>
       </x:c>
-      <x:c r="C15" s="76">
+      <x:c r="C15" s="53">
         <x:v>34684</x:v>
       </x:c>
-      <x:c r="D15" s="76">
+      <x:c r="D15" s="53">
         <x:v>34684</x:v>
       </x:c>
-      <x:c r="E15" s="77" t="s"/>
-      <x:c r="F15" s="77" t="s"/>
-      <x:c r="G15" s="77" t="s">
+      <x:c r="E15" s="51" t="s"/>
+      <x:c r="F15" s="51" t="s"/>
+      <x:c r="G15" s="51" t="s">
         <x:v>23</x:v>
       </x:c>
-      <x:c r="H15" s="78" t="n">
+      <x:c r="H15" s="54" t="n">
         <x:v>1400</x:v>
       </x:c>
-      <x:c r="I15" s="78" t="n">
+      <x:c r="I15" s="54" t="n">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="J15" s="78" t="n">
+      <x:c r="J15" s="54" t="n">
         <x:v>1400</x:v>
       </x:c>
     </x:row>
-    <x:row r="16" spans="1:12" customFormat="1" ht="12" customHeight="1" outlineLevel="2">
+    <x:row r="16" spans="1:11" customFormat="1" ht="12" customHeight="1" outlineLevel="2">
       <x:c r="A16" s="50" t="s"/>
-      <x:c r="B16" s="75" t="n">
+      <x:c r="B16" s="52" t="n">
         <x:v>1169</x:v>
       </x:c>
-      <x:c r="C16" s="76">
+      <x:c r="C16" s="53">
         <x:v>34521</x:v>
       </x:c>
-      <x:c r="D16" s="76">
+      <x:c r="D16" s="53">
         <x:v>34521</x:v>
       </x:c>
-      <x:c r="E16" s="77" t="s"/>
-      <x:c r="F16" s="77" t="s"/>
-      <x:c r="G16" s="77" t="s">
+      <x:c r="E16" s="51" t="s"/>
+      <x:c r="F16" s="51" t="s"/>
+      <x:c r="G16" s="51" t="s">
         <x:v>23</x:v>
       </x:c>
-      <x:c r="H16" s="78" t="n">
+      <x:c r="H16" s="54" t="n">
         <x:v>9471.95</x:v>
       </x:c>
-      <x:c r="I16" s="78" t="n">
+      <x:c r="I16" s="54" t="n">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="J16" s="78" t="n">
+      <x:c r="J16" s="54" t="n">
         <x:v>9471.95</x:v>
       </x:c>
     </x:row>
-    <x:row r="17" spans="1:12" outlineLevel="1">
+    <x:row r="17" spans="1:11" outlineLevel="1">
       <x:c r="A17" s="50" t="s"/>
       <x:c r="B17" s="82" t="s"/>
       <x:c r="C17" s="83" t="s"/>
@@ -1507,59 +1507,59 @@
         <x:f>Subtotal(9,J15:J16)</x:f>
       </x:c>
     </x:row>
-    <x:row r="18" spans="1:12" outlineLevel="2">
+    <x:row r="18" spans="1:11" outlineLevel="2">
       <x:c r="A18" s="50" t="s"/>
-      <x:c r="B18" s="75" t="n">
+      <x:c r="B18" s="52" t="n">
         <x:v>1176</x:v>
       </x:c>
-      <x:c r="C18" s="76">
+      <x:c r="C18" s="53">
         <x:v>34541</x:v>
       </x:c>
-      <x:c r="D18" s="76">
+      <x:c r="D18" s="53">
         <x:v>34541</x:v>
       </x:c>
-      <x:c r="E18" s="77" t="s"/>
-      <x:c r="F18" s="77" t="s"/>
-      <x:c r="G18" s="77" t="s">
+      <x:c r="E18" s="51" t="s"/>
+      <x:c r="F18" s="51" t="s"/>
+      <x:c r="G18" s="51" t="s">
         <x:v>25</x:v>
       </x:c>
-      <x:c r="H18" s="78" t="n">
+      <x:c r="H18" s="54" t="n">
         <x:v>4178.85</x:v>
       </x:c>
-      <x:c r="I18" s="78" t="n">
+      <x:c r="I18" s="54" t="n">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="J18" s="78" t="n">
+      <x:c r="J18" s="54" t="n">
         <x:v>4178.85</x:v>
       </x:c>
     </x:row>
-    <x:row r="19" spans="1:12" outlineLevel="2">
+    <x:row r="19" spans="1:11" outlineLevel="2">
       <x:c r="A19" s="50" t="s"/>
-      <x:c r="B19" s="75" t="n">
+      <x:c r="B19" s="52" t="n">
         <x:v>1076</x:v>
       </x:c>
-      <x:c r="C19" s="76">
+      <x:c r="C19" s="53">
         <x:v>34684</x:v>
       </x:c>
-      <x:c r="D19" s="76">
+      <x:c r="D19" s="53">
         <x:v>32624</x:v>
       </x:c>
-      <x:c r="E19" s="77" t="s"/>
-      <x:c r="F19" s="77" t="s"/>
-      <x:c r="G19" s="77" t="s">
+      <x:c r="E19" s="51" t="s"/>
+      <x:c r="F19" s="51" t="s"/>
+      <x:c r="G19" s="51" t="s">
         <x:v>25</x:v>
       </x:c>
-      <x:c r="H19" s="78" t="n">
+      <x:c r="H19" s="54" t="n">
         <x:v>17781</x:v>
       </x:c>
-      <x:c r="I19" s="78" t="n">
+      <x:c r="I19" s="54" t="n">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="J19" s="78" t="n">
+      <x:c r="J19" s="54" t="n">
         <x:v>17781</x:v>
       </x:c>
     </x:row>
-    <x:row r="20" spans="1:12" outlineLevel="1">
+    <x:row r="20" spans="1:11" outlineLevel="1">
       <x:c r="A20" s="50" t="s"/>
       <x:c r="B20" s="82" t="s"/>
       <x:c r="C20" s="83" t="s"/>
@@ -1577,7 +1577,7 @@
         <x:f>Subtotal(9,J18:J19)</x:f>
       </x:c>
     </x:row>
-    <x:row r="21" spans="1:12">
+    <x:row r="21" spans="1:11">
       <x:c r="A21" s="50" t="s"/>
       <x:c r="B21" s="82" t="s">
         <x:v>27</x:v>
@@ -1595,40 +1595,40 @@
         <x:f>Subtotal(9,J12:J19)</x:f>
       </x:c>
     </x:row>
-    <x:row r="22" spans="1:12">
+    <x:row r="22" spans="1:11">
       <x:c r="A22" s="50" t="s"/>
       <x:c r="B22" s="50" t="s"/>
       <x:c r="C22" s="81" t="s"/>
       <x:c r="D22" s="50" t="s"/>
       <x:c r="E22" s="50" t="s"/>
       <x:c r="F22" s="50" t="s"/>
-      <x:c r="G22" s="55" t="s"/>
+      <x:c r="G22" s="58" t="s"/>
       <x:c r="H22" s="50" t="s"/>
       <x:c r="I22" s="50" t="s"/>
       <x:c r="J22" s="50" t="s"/>
     </x:row>
-    <x:row r="23" spans="1:12">
+    <x:row r="23" spans="1:11">
       <x:c r="A23" s="50" t="s"/>
-      <x:c r="B23" s="56" t="s">
+      <x:c r="B23" s="59" t="s">
         <x:v>28</x:v>
       </x:c>
-      <x:c r="E23" s="56" t="s">
+      <x:c r="E23" s="59" t="s">
         <x:v>29</x:v>
       </x:c>
     </x:row>
-    <x:row r="24" spans="1:12">
+    <x:row r="24" spans="1:11">
       <x:c r="A24" s="50" t="s"/>
       <x:c r="B24" s="80" t="s">
         <x:v>30</x:v>
       </x:c>
-      <x:c r="C24" s="62" t="s"/>
-      <x:c r="D24" s="62" t="s"/>
+      <x:c r="C24" s="66" t="s"/>
+      <x:c r="D24" s="66" t="s"/>
       <x:c r="E24" s="80" t="s">
         <x:v>31</x:v>
       </x:c>
       <x:c r="F24" s="79" t="s"/>
     </x:row>
-    <x:row r="25" spans="1:12">
+    <x:row r="25" spans="1:11">
       <x:c r="G25" s="50" t="s"/>
       <x:c r="H25" s="50" t="s"/>
       <x:c r="I25" s="50" t="s"/>

</xml_diff>